<commit_message>
Include sheet that specifies set of simulation runs defining an experiment, and logic that applies validation to each run's parameter values
</commit_message>
<xml_diff>
--- a/xlsxPCES/examples/embedded-model-exp.xlsx
+++ b/xlsxPCES/examples/embedded-model-exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesbld/xlsxPCES/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2D0A23-735E-F44B-AF56-EC70966D49E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB5BE08B-D49F-2642-972B-4F5AAC96C246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16900" yWindow="2860" windowWidth="29360" windowHeight="18040" activeTab="5" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
+    <workbookView xWindow="5360" yWindow="1120" windowWidth="29360" windowHeight="18040" activeTab="5" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="topo" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="187">
   <si>
     <t>Networks</t>
   </si>
@@ -599,9 +599,6 @@
   </si>
   <si>
     <t>$bndwidth</t>
-  </si>
-  <si>
-    <t>q</t>
   </si>
 </sst>
 </file>
@@ -1574,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95325CDA-052A-9A47-A8FD-348C19C2091E}">
   <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
@@ -1911,7 +1908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FA9935-1338-5743-9994-8B53C9940146}">
   <dimension ref="A3:M101"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A68" zoomScale="150" workbookViewId="0">
       <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
@@ -3457,7 +3454,7 @@
   <dimension ref="A3:D31"/>
   <sheetViews>
     <sheetView zoomScale="98" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3977,24 +3974,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0BE0C2-6CFA-B544-AD1B-E0CD7C820A66}">
-  <dimension ref="A2:E12"/>
+  <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>180</v>
       </c>
@@ -4005,7 +4002,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -4016,7 +4013,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -4027,7 +4024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -4038,7 +4035,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>178</v>
       </c>
@@ -4047,11 +4044,6 @@
       </c>
       <c r="C7" s="12">
         <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E12" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>